<commit_message>
Adding Review form in the form workflow definition
</commit_message>
<xml_diff>
--- a/gms-services/src/main/resources/documentation/drools-form-business-process-rules.xlsx
+++ b/gms-services/src/main/resources/documentation/drools-form-business-process-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GMS\gms-services\src\main\resources\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>RuleSet</t>
   </si>
@@ -243,7 +243,16 @@
     <t>costsheet</t>
   </si>
   <si>
-    <t>New Submission Form</t>
+    <t>submission</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>review</t>
   </si>
 </sst>
 </file>
@@ -891,10 +900,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:G500"/>
+  <dimension ref="A1:G501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,10 +1224,10 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>6</v>
@@ -1235,12 +1244,24 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="5">
+        <v>50</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -5552,6 +5573,15 @@
       <c r="E500" s="5"/>
       <c r="F500" s="5"/>
       <c r="G500" s="5"/>
+    </row>
+    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A501" s="1"/>
+      <c r="B501" s="2"/>
+      <c r="C501" s="6"/>
+      <c r="D501" s="6"/>
+      <c r="E501" s="5"/>
+      <c r="F501" s="5"/>
+      <c r="G501" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>